<commit_message>
ajustes na tradução do game e da task de controle de fases
</commit_message>
<xml_diff>
--- a/scripts/String_15_06_2016_14_08.xlsx
+++ b/scripts/String_15_06_2016_14_08.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6244" uniqueCount="5744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6251" uniqueCount="5751">
   <si>
     <t>Português</t>
   </si>
@@ -31942,6 +31942,28 @@
   </si>
   <si>
     <t>общий</t>
+  </si>
+  <si>
+    <t>Parabéns</t>
+  </si>
+  <si>
+    <t>Congratulations</t>
+  </si>
+  <si>
+    <t>Felicitaciones</t>
+  </si>
+  <si>
+    <t>祝賀</t>
+  </si>
+  <si>
+    <t>تهنئة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Поздравляю</t>
+  </si>
+  <si>
+    <t>Félicitations</t>
   </si>
 </sst>
 </file>
@@ -32590,10 +32612,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1"/>
-  <dimension ref="A1:G892"/>
+  <dimension ref="A1:G893"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B891" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G892" sqref="G892"/>
+      <selection activeCell="G893" sqref="G893"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
@@ -53122,6 +53144,29 @@
       </c>
       <c r="G892" s="3" t="s">
         <v>5740</v>
+      </c>
+    </row>
+    <row r="893" spans="1:7" ht="31.5">
+      <c r="A893" s="3" t="s">
+        <v>5744</v>
+      </c>
+      <c r="B893" s="3" t="s">
+        <v>5745</v>
+      </c>
+      <c r="C893" s="3" t="s">
+        <v>5746</v>
+      </c>
+      <c r="D893" s="3" t="s">
+        <v>5747</v>
+      </c>
+      <c r="E893" s="3" t="s">
+        <v>5748</v>
+      </c>
+      <c r="F893" s="3" t="s">
+        <v>5749</v>
+      </c>
+      <c r="G893" s="3" t="s">
+        <v>5750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>